<commit_message>
Added geometric means bar chart
</commit_message>
<xml_diff>
--- a/Data/DATA_FILE Engineered expression of the invertebrate-specific scorpion toxin AaHIT reduces adult longevity and female fecundity in the diamondback moth Plutella xylostella.xlsx
+++ b/Data/DATA_FILE Engineered expression of the invertebrate-specific scorpion toxin AaHIT reduces adult longevity and female fecundity in the diamondback moth Plutella xylostella.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ueanorwich-my.sharepoint.com/personal/hpd08ucu_uea_ac_uk/Documents/Manuscripts/DBM_analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0358673-BF59-4404-8DEC-42E37A12044A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{E0358673-BF59-4404-8DEC-42E37A12044A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D06DA977-3DC3-4349-B581-33A351E3FBE5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4965" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="22455" yWindow="-3435" windowWidth="12795" windowHeight="6795" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chi-square" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,17 @@
     <sheet name="Figure 5" sheetId="4" r:id="rId4"/>
     <sheet name="Figure 6" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -125,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -959,10 +969,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -1365,7 +1375,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F763"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -16640,16 +16650,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -16657,7 +16667,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -16665,15 +16675,23 @@
         <v>0.13999998799999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3">
         <v>0.110000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <f>(B2+B3+B4)/3</f>
+        <v>0.13333333533333333</v>
+      </c>
+      <c r="D3">
+        <f>GEOMEAN(B2,B3,B4)</f>
+        <v>0.13219164276647824</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -16681,7 +16699,7 @@
         <v>0.15000001399999999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -16689,15 +16707,23 @@
         <v>0.38000000299999998</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6">
         <v>0.58999998399999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <f>(B5+B6+B7)/3</f>
+        <v>0.47333332433333331</v>
+      </c>
+      <c r="D6">
+        <f>GEOMEAN(B5,B6,B7)</f>
+        <v>0.46553181520337672</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -16705,7 +16731,7 @@
         <v>0.44999998600000002</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -16713,15 +16739,23 @@
         <v>0.38000000299999998</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9">
         <v>8.0000002000000001E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <f>(B8+B9+B10)/3</f>
+        <v>0.44000003400000004</v>
+      </c>
+      <c r="D9">
+        <f>GEOMEAN(B8,B9,B10)</f>
+        <v>0.2967955369973066</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -16729,7 +16763,7 @@
         <v>0.86000009700000002</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -16737,15 +16771,31 @@
         <v>2.709999995</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>31</v>
       </c>
       <c r="B12">
         <v>0.60000006900000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <f>(B11+B12+B13+B14)/4</f>
+        <v>1.5025000050000001</v>
+      </c>
+      <c r="D12">
+        <f>GEOMEAN(B11,B12,B13,B14)</f>
+        <v>1.228321766043968</v>
+      </c>
+      <c r="E12">
+        <f>(B11*B12*B13*B14)^(1/3)</f>
+        <v>1.3154758015906818</v>
+      </c>
+      <c r="F12">
+        <f>(B11+B12+B13+B14)/3</f>
+        <v>2.0033333400000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -16753,7 +16803,7 @@
         <v>2.0000000199999999</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -16767,10 +16817,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -17915,7 +17965,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
09/09/20 update ahead of submission - final files.
</commit_message>
<xml_diff>
--- a/Data/DATA_FILE Engineered expression of the invertebrate-specific scorpion toxin AaHIT reduces adult longevity and female fecundity in the diamondback moth Plutella xylostella.xlsx
+++ b/Data/DATA_FILE Engineered expression of the invertebrate-specific scorpion toxin AaHIT reduces adult longevity and female fecundity in the diamondback moth Plutella xylostella.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ueanorwich-my.sharepoint.com/personal/hpd08ucu_uea_ac_uk/Documents/Manuscripts/DBM_analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{E0358673-BF59-4404-8DEC-42E37A12044A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D06DA977-3DC3-4349-B581-33A351E3FBE5}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{E0358673-BF59-4404-8DEC-42E37A12044A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{041D6029-C86A-42FA-8AE4-CA6B3A25A3A6}"/>
   <bookViews>
-    <workbookView xWindow="22455" yWindow="-3435" windowWidth="12795" windowHeight="6795" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4965" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chi-square" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2628" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2646" uniqueCount="40">
   <si>
     <t>Shaking effect</t>
   </si>
@@ -117,19 +117,43 @@
     <t>Lifespan</t>
   </si>
   <si>
-    <t>life_stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relative_quantification_values </t>
-  </si>
-  <si>
     <t>L2</t>
   </si>
   <si>
     <t>L4</t>
   </si>
   <si>
-    <t>3DPE</t>
+    <t>SAMPLE</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>S.E.</t>
+  </si>
+  <si>
+    <t>TET</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>ON-TET</t>
+  </si>
+  <si>
+    <t>1 DPE</t>
+  </si>
+  <si>
+    <t>2 DPE</t>
+  </si>
+  <si>
+    <t>3 DPE</t>
+  </si>
+  <si>
+    <t>4 DPE</t>
+  </si>
+  <si>
+    <t>OFF-TET</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F763"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
@@ -16651,164 +16675,267 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2">
+        <v>0.19</v>
+      </c>
+      <c r="C2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <v>7.2520000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2">
-        <v>0.13999998799999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
       <c r="B3">
-        <v>0.110000004</v>
+        <v>0.37</v>
       </c>
       <c r="C3">
-        <f>(B2+B3+B4)/3</f>
-        <v>0.13333333533333333</v>
-      </c>
-      <c r="D3">
-        <f>GEOMEAN(B2,B3,B4)</f>
-        <v>0.13219164276647824</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3">
+        <v>8.0360000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>0.15000001399999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.12</v>
+      </c>
+      <c r="C4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4">
+        <v>3.5279999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B5">
-        <v>0.38000000299999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.39</v>
+      </c>
+      <c r="C5">
+        <v>0.02</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5">
+        <v>3.9199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B6">
-        <v>0.58999998399999998</v>
+        <v>0.31</v>
       </c>
       <c r="C6">
-        <f>(B5+B6+B7)/3</f>
-        <v>0.47333332433333331</v>
-      </c>
-      <c r="D6">
-        <f>GEOMEAN(B5,B6,B7)</f>
-        <v>0.46553181520337672</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6">
+        <v>0.10192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B7">
-        <v>0.44999998600000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.62</v>
+      </c>
+      <c r="C7">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7">
+        <v>8.0360000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8">
+        <v>0.23</v>
+      </c>
+      <c r="C8">
+        <v>0.105</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8">
+        <v>0.20580000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C9">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9">
+        <v>6.8599999999999994E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>0.47</v>
+      </c>
+      <c r="C10">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10">
+        <v>9.604E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
-        <v>0.38000000299999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9">
-        <v>8.0000002000000001E-2</v>
-      </c>
-      <c r="C9">
-        <f>(B8+B9+B10)/3</f>
-        <v>0.44000003400000004</v>
-      </c>
-      <c r="D9">
-        <f>GEOMEAN(B8,B9,B10)</f>
-        <v>0.2967955369973066</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>0.86000009700000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
       <c r="B11">
-        <v>2.709999995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.3</v>
+      </c>
+      <c r="C11">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11">
+        <v>0.27832000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B12">
-        <v>0.60000006900000002</v>
+        <v>0.82</v>
       </c>
       <c r="C12">
-        <f>(B11+B12+B13+B14)/4</f>
-        <v>1.5025000050000001</v>
-      </c>
-      <c r="D12">
-        <f>GEOMEAN(B11,B12,B13,B14)</f>
-        <v>1.228321766043968</v>
+        <v>0.17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
       </c>
       <c r="E12">
-        <f>(B11*B12*B13*B14)^(1/3)</f>
-        <v>1.3154758015906818</v>
-      </c>
-      <c r="F12">
-        <f>(B11+B12+B13+B14)/3</f>
-        <v>2.0033333400000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.3332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B13">
-        <v>2.0000000199999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1.28</v>
+      </c>
+      <c r="C13">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13">
+        <v>0.54096</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B14">
-        <v>0.69999993599999999</v>
+        <v>1.89</v>
+      </c>
+      <c r="C14">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14">
+        <v>0.45472000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>0.69</v>
+      </c>
+      <c r="C15">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15">
+        <v>8.6239999999999997E-2</v>
       </c>
     </row>
   </sheetData>
@@ -16820,7 +16947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>